<commit_message>
Added RetryAnalyzer, CrossBrowser, Parallel and dataProviders
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -1,43 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakes\git\Repo1\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\newFolder-3\Repo1\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9B7972-EFAF-48A9-A7F1-124DB0A8B118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006A255C-FD61-4E27-AD2F-36A7C39194D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
-    <sheet name="Login" sheetId="3" r:id="rId2"/>
+    <sheet name="login" sheetId="3" r:id="rId2"/>
+    <sheet name="pythonCode" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -127,30 +117,6 @@
   </si>
   <si>
     <t>22777711dd9dfrtfg</t>
-  </si>
-  <si>
-    <t>konikd356</t>
-  </si>
-  <si>
-    <t>lilataghn451</t>
-  </si>
-  <si>
-    <t>janogsd39</t>
-  </si>
-  <si>
-    <t>lipmuio29</t>
-  </si>
-  <si>
-    <t>xersrtdfokokjuhgyh673</t>
-  </si>
-  <si>
-    <t>xswsedrfc589cff</t>
-  </si>
-  <si>
-    <t>bhvgfgfyhu123</t>
-  </si>
-  <si>
-    <t>miok98776</t>
   </si>
   <si>
     <t>Feature File
@@ -161,13 +127,122 @@
   </si>
   <si>
     <t>098zwvsa</t>
+  </si>
+  <si>
+    <t>testtttt</t>
+  </si>
+  <si>
+    <t>testttt</t>
+  </si>
+  <si>
+    <t>ytyutu</t>
+  </si>
+  <si>
+    <t>qachamps3</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Ninjatest@123</t>
+  </si>
+  <si>
+    <t>pythonCode</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\xc
+\xc
+else:
+print("Not Found")
+\xc
+\xc
+\xc
+\xc
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\xc
+\xc
+else:
+count+= 1
+\xc
+\xc
+result = max(result, count)
+\xc
+\xc
+print(result)
+\xc
+\xc
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\xc
+\xc
+\xc
+\xc
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\xc
+\xc
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Some Tests failed. Please review code</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No tests were collected</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +250,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFEBEBEB"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,10 +309,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -205,9 +322,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{DBC3F2C0-FDCB-4F40-91E5-92D8C81EDAEA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -541,11 +673,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3B87CB-D88D-4F0A-BB8F-81BBB5EF62ED}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
@@ -555,7 +687,7 @@
     <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="48.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,10 +702,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
@@ -581,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -592,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -606,7 +738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -623,7 +755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -640,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -657,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -674,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -691,9 +823,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
@@ -708,9 +840,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
@@ -732,19 +864,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5AF72C-2997-422C-89B0-2C3C703E5609}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,36 +884,137 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C1BB72-E077-4E53-9B8E-2362A02F5343}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="180">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="180">
+      <c r="A3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="285">
+      <c r="A4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="285">
+      <c r="A5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="210">
+      <c r="A6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="210">
+      <c r="A7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="180">
+      <c r="A8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="180">
+      <c r="A9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>